<commit_message>
Third and shortest solution
</commit_message>
<xml_diff>
--- a/Excel_Challenge_543 - Top 2 Salaries.xlsx
+++ b/Excel_Challenge_543 - Top 2 Salaries.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7055BA72-CC79-4265-897F-4E870B899024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CE8AE1-EF6A-480B-8101-4DEF32C21E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Alt2" sheetId="4" r:id="rId4"/>
+    <sheet name="Alt3" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$A$1:$C$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$A$1:$C$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Alt3'!$A$1:$C$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$A$1:$C$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$A$1:$C$20</definedName>
   </definedNames>
@@ -67,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="33">
   <si>
     <t>Department</t>
   </si>
@@ -163,6 +165,9 @@
   </si>
   <si>
     <t>Good Use of Array to Text</t>
+  </si>
+  <si>
+    <t>Shortest solution</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02643919-8D5F-4899-B4FC-2B2812DDF01E}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -1994,4 +1999,312 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695CFB09-EC70-491F-8702-E4D158F5DD27}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>921</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>793</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>660</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>579</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="str" cm="1">
+        <f t="array" ref="A24:B27">_xlfn.LET(_xlpm.a,A2:A20,_xlpm.c,C2:C20,_xlfn.GROUPBY(_xlpm.a,B2:B20,_xleta.ARRAYTOTEXT,,0,,COUNTIFS(_xlpm.a,_xlpm.a,_xlpm.c,"&gt;"&amp;_xlpm.c)&lt;2))</f>
+        <v>Admin</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Lauren</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <v>HR</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Thomas, Olivia</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <v>IT</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Emily, Karen, Aaron</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Russell, Lisa</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Trying to break it down further
</commit_message>
<xml_diff>
--- a/Excel_Challenge_543 - Top 2 Salaries.xlsx
+++ b/Excel_Challenge_543 - Top 2 Salaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CE8AE1-EF6A-480B-8101-4DEF32C21E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFDA19D-8F82-4A6D-95F6-3BD00C40DACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -692,6 +692,33 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="792" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{ED38FD4E-5377-4854-8488-C66B914E9738}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
@@ -2005,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695CFB09-EC70-491F-8702-E4D158F5DD27}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2273,7 +2300,19 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="str" cm="1">
-        <f t="array" ref="A24:B27">_xlfn.LET(_xlpm.a,A2:A20,_xlpm.c,C2:C20,_xlfn.GROUPBY(_xlpm.a,B2:B20,_xleta.ARRAYTOTEXT,,0,,COUNTIFS(_xlpm.a,_xlpm.a,_xlpm.c,"&gt;"&amp;_xlpm.c)&lt;2))</f>
+        <f t="array" ref="A24:B27">_xlfn.LET(
+    _xlpm.a, A2:A20,
+    _xlpm.c, C2:C20,
+    _xlfn.GROUPBY(
+        _xlpm.a,
+        B2:B20,
+        _xleta.ARRAYTOTEXT,
+        ,
+        0,
+        ,
+        COUNTIFS(_xlpm.a, _xlpm.a, _xlpm.c, "&gt;" &amp; _xlpm.c) &lt; 2
+    )
+)</f>
         <v>Admin</v>
       </c>
       <c r="B24" t="str">

</xml_diff>